<commit_message>
Agregar excel de datos
</commit_message>
<xml_diff>
--- a/Data/Estimación_de_datos_faltantes.xlsx
+++ b/Data/Estimación_de_datos_faltantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Tesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AA39B9-70E8-4372-B69E-9EC1C773D265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884ABD3D-4E1B-454D-AA14-8D6EA584577C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19242,8 +19242,8 @@
   <dimension ref="A1:I589"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A570" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:B589"/>
+      <pane ySplit="1" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14:D546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34640,7 +34640,7 @@
   <dimension ref="A2:D578"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37052,9 +37052,8 @@
       <c r="C173" s="15">
         <v>0.80967803999999999</v>
       </c>
-      <c r="D173" s="16" t="e">
-        <f>AVERAGE(F173,G173)</f>
-        <v>#DIV/0!</v>
+      <c r="D173" s="16">
+        <v>31.470967741935503</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -38341,9 +38340,8 @@
       <c r="C265" s="15">
         <v>0</v>
       </c>
-      <c r="D265" s="16" t="e">
-        <f>AVERAGE(G265,H265)</f>
-        <v>#DIV/0!</v>
+      <c r="D265" s="16">
+        <v>32.058333333333351</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -41786,9 +41784,8 @@
       <c r="C511" s="15">
         <v>0</v>
       </c>
-      <c r="D511" s="16" t="e">
-        <f>AVERAGE(B511,#REF!,G511)</f>
-        <v>#REF!</v>
+      <c r="D511" s="16">
+        <v>32.569892473118273</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -42060,349 +42057,247 @@
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A531" s="1"/>
       <c r="B531" s="1"/>
-      <c r="C531" s="15">
-        <v>0.86223254999999999</v>
-      </c>
+      <c r="C531" s="15"/>
       <c r="D531" s="15"/>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A532" s="1"/>
       <c r="B532" s="1"/>
-      <c r="C532" s="15">
-        <v>60.757366269999999</v>
-      </c>
+      <c r="C532" s="15"/>
       <c r="D532" s="15"/>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A533" s="1"/>
       <c r="B533" s="1"/>
-      <c r="C533" s="15">
-        <v>132.98436559999999</v>
-      </c>
+      <c r="C533" s="15"/>
       <c r="D533" s="15"/>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A534" s="1"/>
       <c r="B534" s="1"/>
-      <c r="C534" s="15">
-        <v>19.671726530000001</v>
-      </c>
+      <c r="C534" s="15"/>
       <c r="D534" s="15"/>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A535" s="1"/>
       <c r="B535" s="1"/>
-      <c r="C535" s="15">
-        <v>0</v>
-      </c>
+      <c r="C535" s="15"/>
       <c r="D535" s="15"/>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A536" s="1"/>
       <c r="B536" s="1"/>
-      <c r="C536" s="15">
-        <v>0</v>
-      </c>
+      <c r="C536" s="15"/>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A537" s="1"/>
       <c r="B537" s="1"/>
-      <c r="C537" s="15">
-        <v>0</v>
-      </c>
+      <c r="C537" s="15"/>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A538" s="1"/>
       <c r="B538" s="1"/>
-      <c r="C538" s="15">
-        <v>0</v>
-      </c>
+      <c r="C538" s="15"/>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A539" s="1"/>
       <c r="B539" s="1"/>
-      <c r="C539" s="15">
-        <v>0</v>
-      </c>
+      <c r="C539" s="15"/>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A540" s="1"/>
       <c r="B540" s="1"/>
-      <c r="C540" s="15">
-        <v>0</v>
-      </c>
+      <c r="C540" s="15"/>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A541" s="1"/>
       <c r="B541" s="1"/>
-      <c r="C541" s="15">
-        <v>0</v>
-      </c>
+      <c r="C541" s="15"/>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A542" s="1"/>
       <c r="B542" s="1"/>
-      <c r="C542" s="15">
-        <v>0</v>
-      </c>
+      <c r="C542" s="15"/>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A543" s="1"/>
       <c r="B543" s="1"/>
-      <c r="C543" s="10">
-        <v>13.7</v>
-      </c>
+      <c r="C543" s="10"/>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A544" s="1"/>
       <c r="B544" s="1"/>
-      <c r="C544" s="10">
-        <v>24.7</v>
-      </c>
+      <c r="C544" s="10"/>
     </row>
     <row r="545" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A545" s="1"/>
       <c r="B545" s="1"/>
-      <c r="C545" s="10">
-        <v>610.29999999999995</v>
-      </c>
+      <c r="C545" s="10"/>
     </row>
     <row r="546" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A546" s="1"/>
       <c r="B546" s="1"/>
-      <c r="C546" s="10">
-        <v>3</v>
-      </c>
+      <c r="C546" s="10"/>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A547" s="1"/>
       <c r="B547" s="1"/>
-      <c r="C547" s="10">
-        <v>1.5</v>
-      </c>
+      <c r="C547" s="10"/>
     </row>
     <row r="548" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A548" s="1"/>
       <c r="B548" s="1"/>
-      <c r="C548" s="15">
-        <v>0</v>
-      </c>
+      <c r="C548" s="15"/>
     </row>
     <row r="549" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A549" s="1"/>
       <c r="B549" s="1"/>
-      <c r="C549" s="15">
-        <v>0</v>
-      </c>
+      <c r="C549" s="15"/>
     </row>
     <row r="550" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A550" s="1"/>
       <c r="B550" s="1"/>
-      <c r="C550" s="10">
-        <v>0</v>
-      </c>
+      <c r="C550" s="10"/>
     </row>
     <row r="551" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A551" s="1"/>
       <c r="B551" s="1"/>
-      <c r="C551" s="10">
-        <v>0</v>
-      </c>
+      <c r="C551" s="10"/>
     </row>
     <row r="552" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A552" s="1"/>
       <c r="B552" s="1"/>
-      <c r="C552" s="10">
-        <v>0</v>
-      </c>
+      <c r="C552" s="10"/>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A553" s="1"/>
       <c r="B553" s="1"/>
-      <c r="C553" s="10">
-        <v>0</v>
-      </c>
+      <c r="C553" s="10"/>
     </row>
     <row r="554" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A554" s="1"/>
       <c r="B554" s="1"/>
-      <c r="C554" s="15">
-        <v>0</v>
-      </c>
+      <c r="C554" s="15"/>
     </row>
     <row r="555" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A555" s="1"/>
       <c r="B555" s="1"/>
-      <c r="C555" s="15">
-        <v>0.40503650000000002</v>
-      </c>
+      <c r="C555" s="15"/>
     </row>
     <row r="556" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A556" s="1"/>
       <c r="B556" s="1"/>
-      <c r="C556" s="15">
-        <v>0.12732367</v>
-      </c>
+      <c r="C556" s="15"/>
     </row>
     <row r="557" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A557" s="1"/>
       <c r="B557" s="1"/>
-      <c r="C557" s="15">
-        <v>0</v>
-      </c>
+      <c r="C557" s="15"/>
     </row>
     <row r="558" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A558" s="1"/>
       <c r="B558" s="1"/>
-      <c r="C558" s="16" t="e">
-        <f>AVERAGE(#REF!,G558,1)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="C558" s="16"/>
     </row>
     <row r="559" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A559" s="1"/>
       <c r="B559" s="1"/>
-      <c r="C559" s="16" t="e">
-        <f>(#REF!+F559+G559)/4</f>
-        <v>#REF!</v>
-      </c>
+      <c r="C559" s="16"/>
     </row>
     <row r="560" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A560" s="1"/>
       <c r="B560" s="1"/>
-      <c r="C560" s="15">
-        <v>0</v>
-      </c>
+      <c r="C560" s="15"/>
     </row>
     <row r="561" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A561" s="1"/>
       <c r="B561" s="1"/>
-      <c r="C561" s="15">
-        <v>0</v>
-      </c>
+      <c r="C561" s="15"/>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A562" s="1"/>
       <c r="B562" s="1"/>
-      <c r="C562" s="10">
-        <v>0</v>
-      </c>
+      <c r="C562" s="10"/>
     </row>
     <row r="563" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A563" s="1"/>
       <c r="B563" s="1"/>
-      <c r="C563" s="10">
-        <v>0</v>
-      </c>
+      <c r="C563" s="10"/>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A564" s="1"/>
       <c r="B564" s="1"/>
-      <c r="C564" s="10">
-        <v>0</v>
-      </c>
+      <c r="C564" s="10"/>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A565" s="1"/>
       <c r="B565" s="1"/>
-      <c r="C565" s="10">
-        <v>0</v>
-      </c>
+      <c r="C565" s="10"/>
     </row>
     <row r="566" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A566" s="1"/>
       <c r="B566" s="1"/>
-      <c r="C566" s="10">
-        <v>1</v>
-      </c>
+      <c r="C566" s="10"/>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A567" s="1"/>
       <c r="B567" s="1"/>
-      <c r="C567" s="15">
-        <v>1.01635305</v>
-      </c>
+      <c r="C567" s="15"/>
     </row>
     <row r="568" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A568" s="1"/>
       <c r="B568" s="1"/>
-      <c r="C568" s="15">
-        <v>23.235811859999998</v>
-      </c>
+      <c r="C568" s="15"/>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A569" s="1"/>
       <c r="B569" s="1"/>
-      <c r="C569" s="15">
-        <v>3.1546314999999998</v>
-      </c>
+      <c r="C569" s="15"/>
     </row>
     <row r="570" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A570" s="1"/>
       <c r="B570" s="1"/>
-      <c r="C570" s="16" t="e">
-        <f>AVERAGE(D570:G570)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="C570" s="16"/>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A571" s="1"/>
       <c r="B571" s="1"/>
-      <c r="C571" s="10">
-        <v>0</v>
-      </c>
+      <c r="C571" s="10"/>
     </row>
     <row r="572" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A572" s="1"/>
       <c r="B572" s="1"/>
-      <c r="C572" s="10">
-        <v>0</v>
-      </c>
+      <c r="C572" s="10"/>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A573" s="1"/>
       <c r="B573" s="1"/>
-      <c r="C573" s="10">
-        <v>0</v>
-      </c>
+      <c r="C573" s="10"/>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A574" s="1"/>
       <c r="B574" s="1"/>
-      <c r="C574" s="15">
-        <v>0</v>
-      </c>
+      <c r="C574" s="15"/>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A575" s="1"/>
       <c r="B575" s="1"/>
-      <c r="C575" s="10">
-        <v>0</v>
-      </c>
+      <c r="C575" s="10"/>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A576" s="1"/>
       <c r="B576" s="1"/>
-      <c r="C576" s="16" t="e">
-        <f>AVERAGE(#REF!,G576)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="C576" s="16"/>
     </row>
     <row r="577" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A577" s="1"/>
       <c r="B577" s="1"/>
-      <c r="C577" s="16" t="e">
-        <f>AVERAGE(#REF!,G577)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="C577" s="16"/>
     </row>
     <row r="578" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A578" s="1"/>
       <c r="B578" s="1"/>
-      <c r="C578" s="16" t="e">
-        <f>AVERAGE(#REF!,G578)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="C578" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C178">

</xml_diff>